<commit_message>
Added fuel inventories and LHV values
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-biogas.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-biogas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Documents\GitHub\rmnd-lca\rmnd_lca\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5C007E-FF5A-4A40-B957-C59EB8B8C2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CED844-2D96-40C8-A20E-A72161BE4C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF3B9D1A-329E-4EEE-86CA-C40B100D306E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="96">
   <si>
     <t>Activity</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Density: 0.669 kg/Nm3, LHV: 22.6 MJ/kg</t>
+  </si>
+  <si>
+    <t>RU</t>
   </si>
 </sst>
 </file>
@@ -688,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9F37E1-4952-4F96-8F5E-5FDDDA657F4D}">
-  <dimension ref="A1:M294"/>
+  <dimension ref="A1:M319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A288" sqref="A288"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -733,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -960,7 +963,7 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1125,7 +1128,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
         <v>54</v>
@@ -1219,7 +1222,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -1446,7 +1449,7 @@
         <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1602,7 +1605,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B49" s="2">
         <v>0.17937219730941703</v>
@@ -1611,7 +1614,7 @@
         <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E49" t="s">
         <v>54</v>
@@ -1705,7 +1708,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -1932,7 +1935,7 @@
         <v>31</v>
       </c>
       <c r="D68" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2097,7 +2100,7 @@
         <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E74" t="s">
         <v>54</v>
@@ -2191,7 +2194,7 @@
         <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
@@ -2418,7 +2421,7 @@
         <v>31</v>
       </c>
       <c r="D93" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E93" t="s">
         <v>8</v>
@@ -2583,7 +2586,7 @@
         <v>35</v>
       </c>
       <c r="D99" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E99" t="s">
         <v>54</v>
@@ -2677,7 +2680,7 @@
         <v>3</v>
       </c>
       <c r="B105" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.35">
@@ -2904,7 +2907,7 @@
         <v>31</v>
       </c>
       <c r="D118" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E118" t="s">
         <v>8</v>
@@ -3069,7 +3072,7 @@
         <v>35</v>
       </c>
       <c r="D124" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E124" t="s">
         <v>54</v>
@@ -3163,7 +3166,7 @@
         <v>3</v>
       </c>
       <c r="B130" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.35">
@@ -3390,7 +3393,7 @@
         <v>31</v>
       </c>
       <c r="D143" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E143" t="s">
         <v>8</v>
@@ -3555,7 +3558,7 @@
         <v>35</v>
       </c>
       <c r="D149" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E149" t="s">
         <v>54</v>
@@ -3649,7 +3652,7 @@
         <v>3</v>
       </c>
       <c r="B155" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.35">
@@ -3876,7 +3879,7 @@
         <v>31</v>
       </c>
       <c r="D168" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="E168" t="s">
         <v>8</v>
@@ -4041,7 +4044,7 @@
         <v>35</v>
       </c>
       <c r="D174" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="E174" t="s">
         <v>54</v>
@@ -4135,7 +4138,7 @@
         <v>3</v>
       </c>
       <c r="B180" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.35">
@@ -4362,7 +4365,7 @@
         <v>31</v>
       </c>
       <c r="D193" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="E193" t="s">
         <v>8</v>
@@ -4527,7 +4530,7 @@
         <v>35</v>
       </c>
       <c r="D199" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="E199" t="s">
         <v>54</v>
@@ -4621,7 +4624,7 @@
         <v>3</v>
       </c>
       <c r="B205" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.35">
@@ -4848,7 +4851,7 @@
         <v>31</v>
       </c>
       <c r="D218" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E218" t="s">
         <v>8</v>
@@ -5013,7 +5016,7 @@
         <v>35</v>
       </c>
       <c r="D224" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E224" t="s">
         <v>54</v>
@@ -5107,7 +5110,7 @@
         <v>3</v>
       </c>
       <c r="B230" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.35">
@@ -5334,7 +5337,7 @@
         <v>31</v>
       </c>
       <c r="D243" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E243" t="s">
         <v>8</v>
@@ -5499,7 +5502,7 @@
         <v>35</v>
       </c>
       <c r="D249" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E249" t="s">
         <v>54</v>
@@ -5593,7 +5596,7 @@
         <v>3</v>
       </c>
       <c r="B255" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.35">
@@ -5820,7 +5823,7 @@
         <v>31</v>
       </c>
       <c r="D268" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E268" t="s">
         <v>8</v>
@@ -5951,7 +5954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>51</v>
       </c>
@@ -5962,7 +5965,7 @@
         <v>35</v>
       </c>
       <c r="D273" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E273" t="s">
         <v>8</v>
@@ -5974,7 +5977,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>53</v>
       </c>
@@ -5985,7 +5988,7 @@
         <v>35</v>
       </c>
       <c r="D274" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E274" t="s">
         <v>54</v>
@@ -6006,7 +6009,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>59</v>
       </c>
@@ -6035,7 +6038,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>63</v>
       </c>
@@ -6058,23 +6061,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="278" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B279" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>3</v>
       </c>
@@ -6082,7 +6085,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>5</v>
       </c>
@@ -6090,231 +6093,717 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>6</v>
       </c>
       <c r="B282" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>7</v>
       </c>
       <c r="B283" t="s">
         <v>8</v>
       </c>
-      <c r="M283" s="2"/>
-    </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
+        <v>92</v>
+      </c>
+      <c r="B284" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A285" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>10</v>
+      </c>
+      <c r="B286" t="s">
+        <v>11</v>
+      </c>
+      <c r="C286" t="s">
+        <v>12</v>
+      </c>
+      <c r="D286" t="s">
+        <v>3</v>
+      </c>
+      <c r="E286" t="s">
+        <v>7</v>
+      </c>
+      <c r="F286" t="s">
+        <v>13</v>
+      </c>
+      <c r="G286" t="s">
+        <v>14</v>
+      </c>
+      <c r="H286" t="s">
+        <v>15</v>
+      </c>
+      <c r="I286" t="s">
+        <v>2</v>
+      </c>
+      <c r="J286" t="s">
+        <v>6</v>
+      </c>
+      <c r="K286" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>17</v>
+      </c>
+      <c r="B287" s="2">
+        <v>1.8385650224215247E-4</v>
+      </c>
+      <c r="C287" t="s">
+        <v>18</v>
+      </c>
+      <c r="E287" t="s">
+        <v>8</v>
+      </c>
+      <c r="F287" t="s">
+        <v>19</v>
+      </c>
+      <c r="G287" t="s">
+        <v>20</v>
+      </c>
+      <c r="I287" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>22</v>
+      </c>
+      <c r="B288">
+        <v>1.3713596052052344</v>
+      </c>
+      <c r="C288" t="s">
+        <v>18</v>
+      </c>
+      <c r="E288" t="s">
+        <v>8</v>
+      </c>
+      <c r="F288" t="s">
+        <v>19</v>
+      </c>
+      <c r="G288" t="s">
+        <v>20</v>
+      </c>
+      <c r="I288" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>24</v>
+      </c>
+      <c r="B289" s="2">
+        <v>5.2130044843049324E-6</v>
+      </c>
+      <c r="C289" t="s">
+        <v>18</v>
+      </c>
+      <c r="E289" t="s">
+        <v>8</v>
+      </c>
+      <c r="F289" t="s">
+        <v>19</v>
+      </c>
+      <c r="G289" t="s">
+        <v>20</v>
+      </c>
+      <c r="I289" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>26</v>
+      </c>
+      <c r="B290" s="2">
+        <v>4.2869955156950664E-4</v>
+      </c>
+      <c r="C290" t="s">
+        <v>18</v>
+      </c>
+      <c r="E290" t="s">
+        <v>8</v>
+      </c>
+      <c r="F290" t="s">
+        <v>19</v>
+      </c>
+      <c r="G290" t="s">
+        <v>20</v>
+      </c>
+      <c r="H290" t="s">
+        <v>27</v>
+      </c>
+      <c r="I290" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>28</v>
+      </c>
+      <c r="B291" s="2">
+        <v>8.9686098654708509E-6</v>
+      </c>
+      <c r="C291" t="s">
+        <v>18</v>
+      </c>
+      <c r="E291" t="s">
+        <v>8</v>
+      </c>
+      <c r="F291" t="s">
+        <v>19</v>
+      </c>
+      <c r="G291" t="s">
+        <v>20</v>
+      </c>
+      <c r="I291" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>29</v>
+      </c>
+      <c r="B292" s="2">
+        <v>8.2448430493273531E-4</v>
+      </c>
+      <c r="C292" t="s">
+        <v>18</v>
+      </c>
+      <c r="E292" t="s">
+        <v>8</v>
+      </c>
+      <c r="F292" t="s">
+        <v>19</v>
+      </c>
+      <c r="G292" t="s">
+        <v>20</v>
+      </c>
+      <c r="I292" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>1</v>
+      </c>
+      <c r="B293">
+        <v>1</v>
+      </c>
+      <c r="C293" t="s">
+        <v>31</v>
+      </c>
+      <c r="D293" t="s">
+        <v>60</v>
+      </c>
+      <c r="E293" t="s">
+        <v>8</v>
+      </c>
+      <c r="G293" t="s">
+        <v>32</v>
+      </c>
+      <c r="I293" t="s">
+        <v>6</v>
+      </c>
+      <c r="J293" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>34</v>
+      </c>
+      <c r="B294" s="2">
+        <v>2.8160765678334782E-2</v>
+      </c>
+      <c r="C294" t="s">
+        <v>35</v>
+      </c>
+      <c r="D294" t="s">
+        <v>36</v>
+      </c>
+      <c r="E294" t="s">
+        <v>8</v>
+      </c>
+      <c r="G294" t="s">
+        <v>37</v>
+      </c>
+      <c r="I294" t="s">
+        <v>38</v>
+      </c>
+      <c r="J294" t="s">
+        <v>39</v>
+      </c>
+      <c r="K294" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>41</v>
+      </c>
+      <c r="B295" s="2">
+        <v>1.1043437520915599E-3</v>
+      </c>
+      <c r="C295" t="s">
+        <v>35</v>
+      </c>
+      <c r="D295" t="s">
+        <v>36</v>
+      </c>
+      <c r="E295" t="s">
+        <v>8</v>
+      </c>
+      <c r="G295" t="s">
+        <v>37</v>
+      </c>
+      <c r="I295" t="s">
+        <v>42</v>
+      </c>
+      <c r="J295" t="s">
+        <v>43</v>
+      </c>
+      <c r="K295" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>44</v>
+      </c>
+      <c r="B296" s="2">
+        <v>5.9790732436472346E-10</v>
+      </c>
+      <c r="C296" t="s">
+        <v>35</v>
+      </c>
+      <c r="D296" t="s">
+        <v>36</v>
+      </c>
+      <c r="E296" t="s">
+        <v>7</v>
+      </c>
+      <c r="G296" t="s">
+        <v>37</v>
+      </c>
+      <c r="I296" t="s">
+        <v>45</v>
+      </c>
+      <c r="J296" t="s">
+        <v>46</v>
+      </c>
+      <c r="K296" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
+        <v>48</v>
+      </c>
+      <c r="B297" s="2">
+        <v>6.6260625125493598E-5</v>
+      </c>
+      <c r="C297" t="s">
+        <v>35</v>
+      </c>
+      <c r="D297" t="s">
+        <v>36</v>
+      </c>
+      <c r="E297" t="s">
+        <v>8</v>
+      </c>
+      <c r="G297" t="s">
+        <v>37</v>
+      </c>
+      <c r="I297" t="s">
+        <v>49</v>
+      </c>
+      <c r="J297" t="s">
+        <v>50</v>
+      </c>
+      <c r="K297" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
+        <v>51</v>
+      </c>
+      <c r="B298" s="2">
+        <v>6.6260625125493591E-2</v>
+      </c>
+      <c r="C298" t="s">
+        <v>35</v>
+      </c>
+      <c r="D298" t="s">
+        <v>71</v>
+      </c>
+      <c r="E298" t="s">
+        <v>8</v>
+      </c>
+      <c r="G298" t="s">
+        <v>37</v>
+      </c>
+      <c r="J298" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
+        <v>53</v>
+      </c>
+      <c r="B299" s="2">
+        <v>0.17937219730941703</v>
+      </c>
+      <c r="C299" t="s">
+        <v>35</v>
+      </c>
+      <c r="D299" t="s">
+        <v>60</v>
+      </c>
+      <c r="E299" t="s">
+        <v>54</v>
+      </c>
+      <c r="G299" t="s">
+        <v>37</v>
+      </c>
+      <c r="H299" t="s">
+        <v>55</v>
+      </c>
+      <c r="I299" t="s">
+        <v>56</v>
+      </c>
+      <c r="J299" t="s">
+        <v>57</v>
+      </c>
+      <c r="K299" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
+        <v>59</v>
+      </c>
+      <c r="B300" s="2">
+        <v>1.1457566427949933E-2</v>
+      </c>
+      <c r="C300" t="s">
+        <v>31</v>
+      </c>
+      <c r="D300" t="s">
+        <v>60</v>
+      </c>
+      <c r="E300" t="s">
+        <v>8</v>
+      </c>
+      <c r="G300" t="s">
+        <v>37</v>
+      </c>
+      <c r="I300" t="s">
+        <v>61</v>
+      </c>
+      <c r="J300" t="s">
+        <v>62</v>
+      </c>
+      <c r="K300" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
+        <v>63</v>
+      </c>
+      <c r="B301" s="2">
+        <v>2.20868750418312</v>
+      </c>
+      <c r="C301" t="s">
+        <v>35</v>
+      </c>
+      <c r="D301" t="s">
+        <v>4</v>
+      </c>
+      <c r="E301" t="s">
+        <v>64</v>
+      </c>
+      <c r="G301" t="s">
+        <v>37</v>
+      </c>
+      <c r="J301" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A303" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
+        <v>66</v>
+      </c>
+      <c r="B304" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
+        <v>3</v>
+      </c>
+      <c r="B305" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
+        <v>5</v>
+      </c>
+      <c r="B306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>6</v>
+      </c>
+      <c r="B307" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
+        <v>7</v>
+      </c>
+      <c r="B308" t="s">
+        <v>8</v>
+      </c>
+      <c r="M308" s="2"/>
+    </row>
+    <row r="309" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
         <v>68</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B309" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A285" t="s">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
         <v>92</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B310" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="286" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A286" s="1" t="s">
+    <row r="311" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A311" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A287" t="s">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
         <v>10</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B312" t="s">
         <v>11</v>
       </c>
-      <c r="C287" t="s">
+      <c r="C312" t="s">
         <v>12</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D312" t="s">
         <v>3</v>
       </c>
-      <c r="E287" t="s">
+      <c r="E312" t="s">
         <v>7</v>
       </c>
-      <c r="F287" t="s">
+      <c r="F312" t="s">
         <v>14</v>
       </c>
-      <c r="G287" t="s">
+      <c r="G312" t="s">
         <v>69</v>
       </c>
-      <c r="H287" t="s">
+      <c r="H312" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A288" t="s">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
         <v>59</v>
       </c>
-      <c r="B288">
+      <c r="B313">
         <v>1</v>
       </c>
-      <c r="C288" t="s">
+      <c r="C313" t="s">
         <v>31</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D313" t="s">
         <v>60</v>
       </c>
-      <c r="E288" t="s">
-        <v>8</v>
-      </c>
-      <c r="F288" t="s">
+      <c r="E313" t="s">
+        <v>8</v>
+      </c>
+      <c r="F313" t="s">
         <v>32</v>
       </c>
-      <c r="H288" t="s">
+      <c r="H313" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A289" t="s">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
         <v>70</v>
       </c>
-      <c r="B289">
+      <c r="B314">
         <v>2.3800000000000001E-4</v>
       </c>
-      <c r="C289" t="s">
-        <v>35</v>
-      </c>
-      <c r="D289" t="s">
+      <c r="C314" t="s">
+        <v>35</v>
+      </c>
+      <c r="D314" t="s">
         <v>71</v>
       </c>
-      <c r="E289" t="s">
+      <c r="E314" t="s">
         <v>72</v>
       </c>
-      <c r="F289" t="s">
-        <v>37</v>
-      </c>
-      <c r="H289" t="s">
+      <c r="F314" t="s">
+        <v>37</v>
+      </c>
+      <c r="H314" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A290" t="s">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
         <v>74</v>
       </c>
-      <c r="B290">
+      <c r="B315">
         <v>3.4339655648031599E-10</v>
       </c>
-      <c r="C290" t="s">
-        <v>35</v>
-      </c>
-      <c r="D290" t="s">
+      <c r="C315" t="s">
+        <v>35</v>
+      </c>
+      <c r="D315" t="s">
         <v>36</v>
       </c>
-      <c r="E290" t="s">
-        <v>8</v>
-      </c>
-      <c r="F290" t="s">
-        <v>37</v>
-      </c>
-      <c r="G290" t="s">
+      <c r="E315" t="s">
+        <v>8</v>
+      </c>
+      <c r="F315" t="s">
+        <v>37</v>
+      </c>
+      <c r="G315" t="s">
         <v>75</v>
       </c>
-      <c r="H290" t="s">
+      <c r="H315" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A291" t="s">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
         <v>77</v>
       </c>
-      <c r="B291">
+      <c r="B316">
         <v>1.8660000000000003E-2</v>
       </c>
-      <c r="C291" t="s">
-        <v>35</v>
-      </c>
-      <c r="D291" t="s">
+      <c r="C316" t="s">
+        <v>35</v>
+      </c>
+      <c r="D316" t="s">
         <v>36</v>
       </c>
-      <c r="E291" t="s">
-        <v>8</v>
-      </c>
-      <c r="F291" t="s">
-        <v>37</v>
-      </c>
-      <c r="H291" t="s">
+      <c r="E316" t="s">
+        <v>8</v>
+      </c>
+      <c r="F316" t="s">
+        <v>37</v>
+      </c>
+      <c r="H316" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A292" t="s">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
         <v>79</v>
       </c>
-      <c r="B292">
+      <c r="B317">
         <v>8.1000000000000013E-3</v>
       </c>
-      <c r="C292" t="s">
-        <v>35</v>
-      </c>
-      <c r="D292" t="s">
+      <c r="C317" t="s">
+        <v>35</v>
+      </c>
+      <c r="D317" t="s">
         <v>36</v>
       </c>
-      <c r="E292" t="s">
-        <v>8</v>
-      </c>
-      <c r="F292" t="s">
-        <v>37</v>
-      </c>
-      <c r="H292" t="s">
+      <c r="E317" t="s">
+        <v>8</v>
+      </c>
+      <c r="F317" t="s">
+        <v>37</v>
+      </c>
+      <c r="H317" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A293" t="s">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
         <v>51</v>
       </c>
-      <c r="B293">
+      <c r="B318">
         <v>0.996</v>
       </c>
-      <c r="C293" t="s">
-        <v>35</v>
-      </c>
-      <c r="D293" t="s">
+      <c r="C318" t="s">
+        <v>35</v>
+      </c>
+      <c r="D318" t="s">
         <v>71</v>
       </c>
-      <c r="E293" t="s">
-        <v>8</v>
-      </c>
-      <c r="F293" t="s">
-        <v>37</v>
-      </c>
-      <c r="H293" t="s">
+      <c r="E318" t="s">
+        <v>8</v>
+      </c>
+      <c r="F318" t="s">
+        <v>37</v>
+      </c>
+      <c r="H318" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A294" t="s">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
         <v>53</v>
       </c>
-      <c r="B294">
+      <c r="B319">
         <v>3.44E-2</v>
       </c>
-      <c r="C294" t="s">
-        <v>35</v>
-      </c>
-      <c r="D294" t="s">
+      <c r="C319" t="s">
+        <v>35</v>
+      </c>
+      <c r="D319" t="s">
         <v>60</v>
       </c>
-      <c r="E294" t="s">
+      <c r="E319" t="s">
         <v>54</v>
       </c>
-      <c r="F294" t="s">
-        <v>37</v>
-      </c>
-      <c r="H294" t="s">
+      <c r="F319" t="s">
+        <v>37</v>
+      </c>
+      <c r="H319" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>